<commit_message>
add buton click code
</commit_message>
<xml_diff>
--- a/MyFirstApplication/assets/texts/texts.xlsx
+++ b/MyFirstApplication/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1420,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add "-" in text code
</commit_message>
<xml_diff>
--- a/MyFirstApplication/assets/texts/texts.xlsx
+++ b/MyFirstApplication/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="57">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;-&gt;&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&lt;d&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1427,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>53</v>

</xml_diff>